<commit_message>
repull data, push all data, mean calculation
</commit_message>
<xml_diff>
--- a/data/pitcher_data/2022/adam_jason.xlsx
+++ b/data/pitcher_data/2022/adam_jason.xlsx
@@ -66339,7 +66339,7 @@
       </c>
       <c r="F996" t="inlineStr">
         <is>
-          <t>Tim Beckham homers (1) on a fly ball to left center field.   Gilberto Celestino scores.</t>
+          <t>Tim Beckham homers (1) on a fly ball to left center field. Gilberto Celestino scores.</t>
         </is>
       </c>
       <c r="G996" t="inlineStr">
@@ -66408,7 +66408,7 @@
       </c>
       <c r="F997" t="inlineStr">
         <is>
-          <t>Tim Beckham homers (1) on a fly ball to left center field.   Gilberto Celestino scores.</t>
+          <t>Tim Beckham homers (1) on a fly ball to left center field. Gilberto Celestino scores.</t>
         </is>
       </c>
       <c r="G997" t="inlineStr">
@@ -66473,7 +66473,7 @@
       </c>
       <c r="F998" t="inlineStr">
         <is>
-          <t>Tim Beckham homers (1) on a fly ball to left center field.   Gilberto Celestino scores.</t>
+          <t>Tim Beckham homers (1) on a fly ball to left center field. Gilberto Celestino scores.</t>
         </is>
       </c>
       <c r="G998" t="inlineStr">
@@ -66538,7 +66538,7 @@
       </c>
       <c r="F999" t="inlineStr">
         <is>
-          <t>Tim Beckham homers (1) on a fly ball to left center field.   Gilberto Celestino scores.</t>
+          <t>Tim Beckham homers (1) on a fly ball to left center field. Gilberto Celestino scores.</t>
         </is>
       </c>
       <c r="G999" t="inlineStr">
@@ -66603,7 +66603,7 @@
       </c>
       <c r="F1000" t="inlineStr">
         <is>
-          <t>Tim Beckham homers (1) on a fly ball to left center field.   Gilberto Celestino scores.</t>
+          <t>Tim Beckham homers (1) on a fly ball to left center field. Gilberto Celestino scores.</t>
         </is>
       </c>
       <c r="G1000" t="inlineStr">
@@ -66668,7 +66668,7 @@
       </c>
       <c r="F1001" t="inlineStr">
         <is>
-          <t>Tim Beckham homers (1) on a fly ball to left center field.   Gilberto Celestino scores.</t>
+          <t>Tim Beckham homers (1) on a fly ball to left center field. Gilberto Celestino scores.</t>
         </is>
       </c>
       <c r="G1001" t="inlineStr">

</xml_diff>